<commit_message>
Image added in the PDF file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\InPhase_Electronics\Desktop\01_04_24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A079F44B-E429-4EB2-B5D4-D465976C4DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12C1286-ADF0-46E6-B17F-F4E31361D01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{984A1824-DFFF-44F2-A0D8-540C9BE01F30}"/>
   </bookViews>
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08081D88-E500-4ED5-8FA9-630EA4E64C41}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A31" sqref="A31:A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,6 +1011,456 @@
         <v>4353</v>
       </c>
     </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7">
+        <v>150</v>
+      </c>
+      <c r="C32" s="7">
+        <v>7654</v>
+      </c>
+      <c r="D32" s="7">
+        <f>AVERAGE(B32:C32)</f>
+        <v>3902</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7">
+        <v>160</v>
+      </c>
+      <c r="C33" s="7">
+        <v>4567</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" ref="D33:D61" si="1">AVERAGE(B33:C33)</f>
+        <v>2363.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7">
+        <v>170</v>
+      </c>
+      <c r="C34" s="7">
+        <v>9876</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="1"/>
+        <v>5023</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7">
+        <v>180</v>
+      </c>
+      <c r="C35" s="7">
+        <v>5432</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="1"/>
+        <v>2806</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7">
+        <v>190</v>
+      </c>
+      <c r="C36" s="7">
+        <v>6543</v>
+      </c>
+      <c r="D36" s="7">
+        <f t="shared" si="1"/>
+        <v>3366.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7">
+        <v>200</v>
+      </c>
+      <c r="C37" s="7">
+        <v>8764</v>
+      </c>
+      <c r="D37" s="7">
+        <f t="shared" si="1"/>
+        <v>4482</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7">
+        <v>210</v>
+      </c>
+      <c r="C38" s="7">
+        <v>9876</v>
+      </c>
+      <c r="D38" s="7">
+        <f t="shared" si="1"/>
+        <v>5043</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7">
+        <v>220</v>
+      </c>
+      <c r="C39" s="7">
+        <v>3456</v>
+      </c>
+      <c r="D39" s="7">
+        <f t="shared" si="1"/>
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7">
+        <v>230</v>
+      </c>
+      <c r="C40" s="7">
+        <v>6545</v>
+      </c>
+      <c r="D40" s="7">
+        <f t="shared" si="1"/>
+        <v>3387.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7">
+        <v>240</v>
+      </c>
+      <c r="C41" s="7">
+        <v>1234</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" si="1"/>
+        <v>737</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7">
+        <v>250</v>
+      </c>
+      <c r="C42" s="7">
+        <v>6432</v>
+      </c>
+      <c r="D42" s="7">
+        <f t="shared" si="1"/>
+        <v>3341</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7">
+        <v>260</v>
+      </c>
+      <c r="C43" s="7">
+        <v>9786</v>
+      </c>
+      <c r="D43" s="7">
+        <f t="shared" si="1"/>
+        <v>5023</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7">
+        <v>270</v>
+      </c>
+      <c r="C44" s="7">
+        <v>8977</v>
+      </c>
+      <c r="D44" s="7">
+        <f t="shared" si="1"/>
+        <v>4623.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7">
+        <v>280</v>
+      </c>
+      <c r="C45" s="7">
+        <v>3456</v>
+      </c>
+      <c r="D45" s="7">
+        <f t="shared" si="1"/>
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7">
+        <v>290</v>
+      </c>
+      <c r="C46" s="7">
+        <v>7866</v>
+      </c>
+      <c r="D46" s="7">
+        <f t="shared" si="1"/>
+        <v>4078</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7">
+        <v>300</v>
+      </c>
+      <c r="C47" s="7">
+        <v>5353</v>
+      </c>
+      <c r="D47" s="7">
+        <f t="shared" si="1"/>
+        <v>2826.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7">
+        <v>310</v>
+      </c>
+      <c r="C48" s="7">
+        <v>7564</v>
+      </c>
+      <c r="D48" s="7">
+        <f t="shared" si="1"/>
+        <v>3937</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7">
+        <v>320</v>
+      </c>
+      <c r="C49" s="7">
+        <v>4738</v>
+      </c>
+      <c r="D49" s="7">
+        <f t="shared" si="1"/>
+        <v>2529</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7">
+        <v>330</v>
+      </c>
+      <c r="C50" s="7">
+        <v>2468</v>
+      </c>
+      <c r="D50" s="7">
+        <f t="shared" si="1"/>
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7">
+        <v>340</v>
+      </c>
+      <c r="C51" s="7">
+        <v>8346</v>
+      </c>
+      <c r="D51" s="7">
+        <f t="shared" si="1"/>
+        <v>4343</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7">
+        <v>341</v>
+      </c>
+      <c r="C52" s="7">
+        <v>8347</v>
+      </c>
+      <c r="D52" s="7">
+        <f t="shared" si="1"/>
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>52</v>
+      </c>
+      <c r="B53" s="7">
+        <v>342</v>
+      </c>
+      <c r="C53" s="7">
+        <v>8348</v>
+      </c>
+      <c r="D53" s="7">
+        <f t="shared" si="1"/>
+        <v>4345</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>53</v>
+      </c>
+      <c r="B54" s="7">
+        <v>343</v>
+      </c>
+      <c r="C54" s="7">
+        <v>8349</v>
+      </c>
+      <c r="D54" s="7">
+        <f t="shared" si="1"/>
+        <v>4346</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>54</v>
+      </c>
+      <c r="B55" s="7">
+        <v>344</v>
+      </c>
+      <c r="C55" s="7">
+        <v>8350</v>
+      </c>
+      <c r="D55" s="7">
+        <f t="shared" si="1"/>
+        <v>4347</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>55</v>
+      </c>
+      <c r="B56" s="7">
+        <v>345</v>
+      </c>
+      <c r="C56" s="7">
+        <v>8351</v>
+      </c>
+      <c r="D56" s="7">
+        <f t="shared" si="1"/>
+        <v>4348</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>56</v>
+      </c>
+      <c r="B57" s="7">
+        <v>346</v>
+      </c>
+      <c r="C57" s="7">
+        <v>8352</v>
+      </c>
+      <c r="D57" s="7">
+        <f t="shared" si="1"/>
+        <v>4349</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>57</v>
+      </c>
+      <c r="B58" s="7">
+        <v>347</v>
+      </c>
+      <c r="C58" s="7">
+        <v>8353</v>
+      </c>
+      <c r="D58" s="7">
+        <f t="shared" si="1"/>
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>58</v>
+      </c>
+      <c r="B59" s="7">
+        <v>348</v>
+      </c>
+      <c r="C59" s="7">
+        <v>8354</v>
+      </c>
+      <c r="D59" s="7">
+        <f t="shared" si="1"/>
+        <v>4351</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>59</v>
+      </c>
+      <c r="B60" s="7">
+        <v>349</v>
+      </c>
+      <c r="C60" s="7">
+        <v>8355</v>
+      </c>
+      <c r="D60" s="7">
+        <f t="shared" si="1"/>
+        <v>4352</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>60</v>
+      </c>
+      <c r="B61" s="7">
+        <v>350</v>
+      </c>
+      <c r="C61" s="7">
+        <v>8356</v>
+      </c>
+      <c r="D61" s="7">
+        <f t="shared" si="1"/>
+        <v>4353</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>